<commit_message>
perbaikan minor fungsi, testing bot ke line
</commit_message>
<xml_diff>
--- a/tabel db.xlsx
+++ b/tabel db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\ITB\PPLJ (Perancangan Perangkat Lunak Jaringan)\Tubes\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F4ABEA4-3D70-4D37-A72A-C5455E912EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61097EF0-1C36-4A00-B9C0-F900A73DE1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="1560" windowWidth="13824" windowHeight="9852" xr2:uid="{E1FB495C-DA11-4B93-A0F9-F12DC51F8976}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1FB495C-DA11-4B93-A0F9-F12DC51F8976}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>tabel utang</t>
   </si>
@@ -48,9 +48,6 @@
     <t>kevin</t>
   </si>
   <si>
-    <t>price</t>
-  </si>
-  <si>
     <t>daftar command</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>id_lender</t>
   </si>
   <si>
-    <t>id_debtor</t>
-  </si>
-  <si>
     <t>nomor</t>
   </si>
   <si>
@@ -120,10 +114,28 @@
     <t>sebas</t>
   </si>
   <si>
-    <t>confirmed</t>
-  </si>
-  <si>
     <t>ari</t>
+  </si>
+  <si>
+    <t>id_borrower</t>
+  </si>
+  <si>
+    <t>harga</t>
+  </si>
+  <si>
+    <t>konfirmasi</t>
+  </si>
+  <si>
+    <t>Tabel User</t>
+  </si>
+  <si>
+    <t>Tabel Utang</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>timestamp</t>
   </si>
 </sst>
 </file>
@@ -147,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -170,17 +182,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -188,7 +189,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -553,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51DACD9-667B-463E-BDB5-CAAC2B848A17}">
-  <dimension ref="A2:I16"/>
+  <dimension ref="A2:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,52 +565,84 @@
     <col min="1" max="1" width="3.21875" customWidth="1"/>
     <col min="2" max="2" width="37.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -620,13 +653,19 @@
       <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -635,15 +674,21 @@
         <v>12345</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -652,15 +697,21 @@
         <v>123456</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="K7" s="1">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3">
         <v>4</v>
@@ -669,66 +720,123 @@
         <v>123</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="K8" s="3">
+        <v>4</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="I11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="L12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="P12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C13" s="1">
         <v>1</v>
       </c>
@@ -736,7 +844,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1">
@@ -744,8 +852,18 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
         <v>2</v>
       </c>
@@ -753,7 +871,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1">
@@ -761,13 +879,23 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K14" s="1">
+        <v>2</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C15" s="1">
         <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>3</v>
@@ -778,17 +906,41 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="K15" s="1">
         <v>3</v>
       </c>
-      <c r="G16" s="2">
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C16" s="1"/>
+      <c r="D16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="3">
         <v>8</v>
       </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="K16" s="1">
+        <v>4</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>